<commit_message>
update lots of things
</commit_message>
<xml_diff>
--- a/autolist2.0.xlsx
+++ b/autolist2.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\WorkSpace3\HPEasyShell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F754BB47-DF75-48BD-BD35-19247BC74D58}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC11466-04C7-4CFD-B33B-283C3027C5D6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="241">
   <si>
     <t>Feature</t>
   </si>
@@ -752,18 +752,43 @@
   </si>
   <si>
     <t>Shutdown, logoff会影响测试</t>
+  </si>
+  <si>
+    <t>kiosk_onoff</t>
+  </si>
+  <si>
+    <t>easyshell_launch</t>
+  </si>
+  <si>
+    <t>wifi_readonly</t>
+  </si>
+  <si>
+    <t>wifi_modify_settings</t>
+  </si>
+  <si>
+    <t>wifi_modify_icon</t>
+  </si>
+  <si>
+    <t>wifi_wpap</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -893,7 +918,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -943,22 +968,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -976,10 +1001,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -991,10 +1016,10 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1007,19 +1032,25 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1312,21 +1343,21 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I136"/>
+  <dimension ref="A1:I137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B38" sqref="B38"/>
+      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D98" sqref="D98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2" style="37" customWidth="1"/>
     <col min="2" max="2" width="95.42578125" style="37" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" style="37" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="0.42578125" style="27" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="0.5703125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" customWidth="1"/>
     <col min="7" max="7" width="79.42578125" style="37" customWidth="1"/>
     <col min="8" max="16384" width="9" style="37"/>
   </cols>
@@ -1358,7 +1389,7 @@
       </c>
       <c r="I1" s="36"/>
     </row>
-    <row r="2" spans="1:9" customFormat="1" hidden="1">
+    <row r="2" spans="1:9" customFormat="1" ht="210" hidden="1">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1404,7 +1435,7 @@
       </c>
       <c r="I3" s="8"/>
     </row>
-    <row r="4" spans="1:9" hidden="1">
+    <row r="4" spans="1:9">
       <c r="A4" s="30"/>
       <c r="B4" s="30" t="s">
         <v>13</v>
@@ -1421,7 +1452,9 @@
       <c r="F4" s="4">
         <v>0</v>
       </c>
-      <c r="G4" s="30"/>
+      <c r="G4" s="40" t="s">
+        <v>215</v>
+      </c>
       <c r="H4" s="38"/>
       <c r="I4" s="36"/>
     </row>
@@ -1555,7 +1588,7 @@
       <c r="H10" s="3"/>
       <c r="I10" s="8"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" hidden="1">
       <c r="A11" s="5"/>
       <c r="B11" s="5" t="s">
         <v>26</v>
@@ -1576,7 +1609,7 @@
       <c r="H11" s="38"/>
       <c r="I11" s="36"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" hidden="1">
       <c r="A12" s="5"/>
       <c r="B12" s="5" t="s">
         <v>28</v>
@@ -1618,7 +1651,7 @@
       <c r="H13" s="3"/>
       <c r="I13" s="8"/>
     </row>
-    <row r="14" spans="1:9" customFormat="1" hidden="1">
+    <row r="14" spans="1:9" customFormat="1" ht="315" hidden="1">
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
@@ -1662,7 +1695,7 @@
       <c r="H15" s="3"/>
       <c r="I15" s="8"/>
     </row>
-    <row r="16" spans="1:9" hidden="1">
+    <row r="16" spans="1:9">
       <c r="A16" s="30"/>
       <c r="B16" s="30" t="s">
         <v>36</v>
@@ -1677,7 +1710,9 @@
       <c r="F16" s="6">
         <v>0</v>
       </c>
-      <c r="G16" s="30"/>
+      <c r="G16" s="40" t="s">
+        <v>215</v>
+      </c>
       <c r="H16" s="38"/>
       <c r="I16" s="36"/>
     </row>
@@ -1702,7 +1737,7 @@
       <c r="H17" s="3"/>
       <c r="I17" s="8"/>
     </row>
-    <row r="18" spans="1:9" ht="30">
+    <row r="18" spans="1:9" ht="30" hidden="1">
       <c r="A18" s="5"/>
       <c r="B18" s="5" t="s">
         <v>39</v>
@@ -1723,7 +1758,7 @@
       <c r="H18" s="38"/>
       <c r="I18" s="36"/>
     </row>
-    <row r="19" spans="1:9" ht="30">
+    <row r="19" spans="1:9" ht="30" hidden="1">
       <c r="A19" s="7"/>
       <c r="B19" s="7" t="s">
         <v>40</v>
@@ -1744,7 +1779,7 @@
       <c r="H19" s="38"/>
       <c r="I19" s="36"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" hidden="1">
       <c r="A20" s="5"/>
       <c r="B20" s="5" t="s">
         <v>41</v>
@@ -1765,7 +1800,7 @@
       <c r="H20" s="38"/>
       <c r="I20" s="36"/>
     </row>
-    <row r="21" spans="1:9" ht="30" hidden="1">
+    <row r="21" spans="1:9" ht="27" customHeight="1">
       <c r="A21" s="30" t="s">
         <v>42</v>
       </c>
@@ -1788,7 +1823,7 @@
       <c r="H21" s="38"/>
       <c r="I21" s="36"/>
     </row>
-    <row r="22" spans="1:9" ht="30">
+    <row r="22" spans="1:9" ht="30" hidden="1">
       <c r="A22" s="5"/>
       <c r="B22" s="5" t="s">
         <v>44</v>
@@ -1809,7 +1844,7 @@
       <c r="H22" s="38"/>
       <c r="I22" s="36"/>
     </row>
-    <row r="23" spans="1:9" ht="30" hidden="1">
+    <row r="23" spans="1:9" ht="30">
       <c r="A23" s="30"/>
       <c r="B23" s="30" t="s">
         <v>45</v>
@@ -1830,7 +1865,7 @@
       <c r="H23" s="38"/>
       <c r="I23" s="36"/>
     </row>
-    <row r="24" spans="1:9" ht="30" hidden="1">
+    <row r="24" spans="1:9" ht="30">
       <c r="A24" s="30"/>
       <c r="B24" s="30" t="s">
         <v>46</v>
@@ -1851,7 +1886,7 @@
       <c r="H24" s="38"/>
       <c r="I24" s="36"/>
     </row>
-    <row r="25" spans="1:9" ht="30" hidden="1">
+    <row r="25" spans="1:9" ht="30">
       <c r="A25" s="30"/>
       <c r="B25" s="30" t="s">
         <v>47</v>
@@ -1872,7 +1907,7 @@
       <c r="H25" s="38"/>
       <c r="I25" s="36"/>
     </row>
-    <row r="26" spans="1:9" ht="30" hidden="1">
+    <row r="26" spans="1:9" ht="30">
       <c r="A26" s="30"/>
       <c r="B26" s="30" t="s">
         <v>48</v>
@@ -1893,7 +1928,7 @@
       <c r="H26" s="38"/>
       <c r="I26" s="36"/>
     </row>
-    <row r="27" spans="1:9" ht="30" hidden="1">
+    <row r="27" spans="1:9" ht="30">
       <c r="A27" s="30"/>
       <c r="B27" s="30" t="s">
         <v>49</v>
@@ -1914,7 +1949,7 @@
       <c r="H27" s="38"/>
       <c r="I27" s="36"/>
     </row>
-    <row r="28" spans="1:9" ht="30" hidden="1">
+    <row r="28" spans="1:9" ht="30">
       <c r="A28" s="30"/>
       <c r="B28" s="30" t="s">
         <v>50</v>
@@ -1935,7 +1970,7 @@
       <c r="H28" s="38"/>
       <c r="I28" s="36"/>
     </row>
-    <row r="29" spans="1:9" ht="30">
+    <row r="29" spans="1:9" ht="30" hidden="1">
       <c r="A29" s="5"/>
       <c r="B29" s="5" t="s">
         <v>51</v>
@@ -1956,7 +1991,7 @@
       <c r="H29" s="38"/>
       <c r="I29" s="36"/>
     </row>
-    <row r="30" spans="1:9" ht="30">
+    <row r="30" spans="1:9" ht="30" hidden="1">
       <c r="A30" s="5"/>
       <c r="B30" s="5" t="s">
         <v>52</v>
@@ -1977,7 +2012,7 @@
       <c r="H30" s="38"/>
       <c r="I30" s="36"/>
     </row>
-    <row r="31" spans="1:9" customFormat="1" hidden="1">
+    <row r="31" spans="1:9" customFormat="1" ht="90" hidden="1">
       <c r="A31" s="1" t="s">
         <v>53</v>
       </c>
@@ -2021,7 +2056,7 @@
       <c r="H32" s="3"/>
       <c r="I32" s="8"/>
     </row>
-    <row r="33" spans="1:9" hidden="1">
+    <row r="33" spans="1:9">
       <c r="A33" s="30"/>
       <c r="B33" s="30" t="s">
         <v>58</v>
@@ -2036,7 +2071,9 @@
       <c r="F33" s="6">
         <v>0</v>
       </c>
-      <c r="G33" s="39"/>
+      <c r="G33" s="40" t="s">
+        <v>215</v>
+      </c>
       <c r="H33" s="38"/>
       <c r="I33" s="36"/>
     </row>
@@ -2061,7 +2098,7 @@
       <c r="H34" s="3"/>
       <c r="I34" s="8"/>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" hidden="1">
       <c r="A35" s="5"/>
       <c r="B35" s="5" t="s">
         <v>61</v>
@@ -2082,7 +2119,7 @@
       <c r="H35" s="38"/>
       <c r="I35" s="36"/>
     </row>
-    <row r="36" spans="1:9" ht="30">
+    <row r="36" spans="1:9" ht="30" hidden="1">
       <c r="A36" s="5"/>
       <c r="B36" s="5" t="s">
         <v>62</v>
@@ -2103,7 +2140,7 @@
       <c r="H36" s="38"/>
       <c r="I36" s="36"/>
     </row>
-    <row r="37" spans="1:9" hidden="1">
+    <row r="37" spans="1:9">
       <c r="A37" s="30"/>
       <c r="B37" s="30" t="s">
         <v>63</v>
@@ -2124,7 +2161,7 @@
       <c r="H37" s="38"/>
       <c r="I37" s="36"/>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" hidden="1">
       <c r="A38" s="5"/>
       <c r="B38" s="5" t="s">
         <v>64</v>
@@ -2145,7 +2182,7 @@
       <c r="H38" s="38"/>
       <c r="I38" s="36"/>
     </row>
-    <row r="39" spans="1:9" customFormat="1" hidden="1">
+    <row r="39" spans="1:9" customFormat="1" ht="195" hidden="1">
       <c r="A39" s="1" t="s">
         <v>65</v>
       </c>
@@ -2189,7 +2226,7 @@
       <c r="H40" s="3"/>
       <c r="I40" s="8"/>
     </row>
-    <row r="41" spans="1:9" hidden="1">
+    <row r="41" spans="1:9">
       <c r="A41" s="30"/>
       <c r="B41" s="30" t="s">
         <v>70</v>
@@ -2231,7 +2268,7 @@
       <c r="H42" s="3"/>
       <c r="I42" s="8"/>
     </row>
-    <row r="43" spans="1:9" hidden="1">
+    <row r="43" spans="1:9">
       <c r="A43" s="30"/>
       <c r="B43" s="30" t="s">
         <v>73</v>
@@ -2252,7 +2289,7 @@
       <c r="H43" s="38"/>
       <c r="I43" s="36"/>
     </row>
-    <row r="44" spans="1:9" hidden="1">
+    <row r="44" spans="1:9">
       <c r="A44" s="30"/>
       <c r="B44" s="30" t="s">
         <v>74</v>
@@ -2273,7 +2310,7 @@
       <c r="H44" s="38"/>
       <c r="I44" s="36"/>
     </row>
-    <row r="45" spans="1:9" hidden="1">
+    <row r="45" spans="1:9">
       <c r="A45" s="30"/>
       <c r="B45" s="30" t="s">
         <v>75</v>
@@ -2294,7 +2331,7 @@
       <c r="H45" s="38"/>
       <c r="I45" s="36"/>
     </row>
-    <row r="46" spans="1:9" ht="30">
+    <row r="46" spans="1:9" ht="30" hidden="1">
       <c r="A46" s="5"/>
       <c r="B46" s="5" t="s">
         <v>76</v>
@@ -2315,7 +2352,7 @@
       <c r="H46" s="38"/>
       <c r="I46" s="36"/>
     </row>
-    <row r="47" spans="1:9" hidden="1">
+    <row r="47" spans="1:9">
       <c r="A47" s="30"/>
       <c r="B47" s="30" t="s">
         <v>77</v>
@@ -2336,7 +2373,7 @@
       <c r="H47" s="38"/>
       <c r="I47" s="36"/>
     </row>
-    <row r="48" spans="1:9" hidden="1">
+    <row r="48" spans="1:9">
       <c r="A48" s="30"/>
       <c r="B48" s="30" t="s">
         <v>78</v>
@@ -2357,7 +2394,7 @@
       <c r="H48" s="38"/>
       <c r="I48" s="36"/>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" hidden="1">
       <c r="A49" s="5"/>
       <c r="B49" s="5" t="s">
         <v>79</v>
@@ -2378,7 +2415,7 @@
       <c r="H49" s="38"/>
       <c r="I49" s="36"/>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" hidden="1">
       <c r="A50" s="5"/>
       <c r="B50" s="5" t="s">
         <v>80</v>
@@ -2399,7 +2436,7 @@
       <c r="H50" s="38"/>
       <c r="I50" s="36"/>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" hidden="1">
       <c r="A51" s="5"/>
       <c r="B51" s="5" t="s">
         <v>81</v>
@@ -2420,7 +2457,7 @@
       <c r="H51" s="38"/>
       <c r="I51" s="36"/>
     </row>
-    <row r="52" spans="1:9" hidden="1">
+    <row r="52" spans="1:9">
       <c r="A52" s="30"/>
       <c r="B52" s="30" t="s">
         <v>82</v>
@@ -2441,7 +2478,7 @@
       <c r="H52" s="38"/>
       <c r="I52" s="36"/>
     </row>
-    <row r="53" spans="1:9" hidden="1">
+    <row r="53" spans="1:9">
       <c r="A53" s="30"/>
       <c r="B53" s="30" t="s">
         <v>83</v>
@@ -2462,7 +2499,7 @@
       <c r="H53" s="38"/>
       <c r="I53" s="36"/>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" hidden="1">
       <c r="A54" s="5"/>
       <c r="B54" s="5" t="s">
         <v>84</v>
@@ -2483,19 +2520,19 @@
       <c r="H54" s="38"/>
       <c r="I54" s="36"/>
     </row>
-    <row r="55" spans="1:9" hidden="1">
+    <row r="55" spans="1:9">
       <c r="A55" s="30"/>
       <c r="B55" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="C55" s="2"/>
+      <c r="C55" s="30"/>
       <c r="D55" s="30" t="s">
         <v>212</v>
       </c>
       <c r="E55" s="25">
         <v>2</v>
       </c>
-      <c r="F55" s="2">
+      <c r="F55" s="30">
         <v>3</v>
       </c>
       <c r="G55" s="40" t="s">
@@ -2504,19 +2541,19 @@
       <c r="H55" s="38"/>
       <c r="I55" s="36"/>
     </row>
-    <row r="56" spans="1:9" hidden="1">
+    <row r="56" spans="1:9">
       <c r="A56" s="30"/>
       <c r="B56" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="C56" s="2"/>
+      <c r="C56" s="30"/>
       <c r="D56" s="30" t="s">
         <v>212</v>
       </c>
       <c r="E56" s="25">
         <v>2</v>
       </c>
-      <c r="F56" s="2">
+      <c r="F56" s="30">
         <v>3</v>
       </c>
       <c r="G56" s="40" t="s">
@@ -2525,19 +2562,19 @@
       <c r="H56" s="38"/>
       <c r="I56" s="36"/>
     </row>
-    <row r="57" spans="1:9" hidden="1">
+    <row r="57" spans="1:9">
       <c r="A57" s="30"/>
       <c r="B57" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="C57" s="2"/>
+      <c r="C57" s="30"/>
       <c r="D57" s="30" t="s">
         <v>212</v>
       </c>
       <c r="E57" s="25">
         <v>2</v>
       </c>
-      <c r="F57" s="2">
+      <c r="F57" s="30">
         <v>2</v>
       </c>
       <c r="G57" s="40" t="s">
@@ -2546,7 +2583,7 @@
       <c r="H57" s="38"/>
       <c r="I57" s="36"/>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" hidden="1">
       <c r="A58" s="5"/>
       <c r="B58" s="5" t="s">
         <v>88</v>
@@ -2567,7 +2604,7 @@
       <c r="H58" s="38"/>
       <c r="I58" s="36"/>
     </row>
-    <row r="59" spans="1:9" customFormat="1" hidden="1">
+    <row r="59" spans="1:9" customFormat="1" ht="195" hidden="1">
       <c r="A59" s="1" t="s">
         <v>89</v>
       </c>
@@ -2611,22 +2648,24 @@
       <c r="H60" s="3"/>
       <c r="I60" s="8"/>
     </row>
-    <row r="61" spans="1:9" hidden="1">
+    <row r="61" spans="1:9">
       <c r="A61" s="30"/>
       <c r="B61" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="C61" s="6"/>
+      <c r="C61" s="30"/>
       <c r="D61" s="30" t="s">
         <v>212</v>
       </c>
       <c r="E61" s="24">
         <v>2</v>
       </c>
-      <c r="F61" s="6">
+      <c r="F61" s="30">
         <v>0</v>
       </c>
-      <c r="G61" s="39"/>
+      <c r="G61" s="40" t="s">
+        <v>215</v>
+      </c>
       <c r="H61" s="38"/>
       <c r="I61" s="36"/>
     </row>
@@ -2651,19 +2690,19 @@
       <c r="H62" s="3"/>
       <c r="I62" s="8"/>
     </row>
-    <row r="63" spans="1:9" hidden="1">
+    <row r="63" spans="1:9">
       <c r="A63" s="30"/>
       <c r="B63" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="C63" s="6"/>
+      <c r="C63" s="30"/>
       <c r="D63" s="30" t="s">
         <v>212</v>
       </c>
       <c r="E63" s="24">
         <v>2</v>
       </c>
-      <c r="F63" s="6">
+      <c r="F63" s="30">
         <v>2</v>
       </c>
       <c r="G63" s="40" t="s">
@@ -2672,19 +2711,19 @@
       <c r="H63" s="38"/>
       <c r="I63" s="36"/>
     </row>
-    <row r="64" spans="1:9" hidden="1">
+    <row r="64" spans="1:9">
       <c r="A64" s="30"/>
       <c r="B64" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="C64" s="6"/>
+      <c r="C64" s="30"/>
       <c r="D64" s="30" t="s">
         <v>212</v>
       </c>
       <c r="E64" s="24">
         <v>2</v>
       </c>
-      <c r="F64" s="6">
+      <c r="F64" s="30">
         <v>2</v>
       </c>
       <c r="G64" s="40" t="s">
@@ -2693,7 +2732,7 @@
       <c r="H64" s="38"/>
       <c r="I64" s="36"/>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" hidden="1">
       <c r="A65" s="5"/>
       <c r="B65" s="5" t="s">
         <v>99</v>
@@ -2714,7 +2753,7 @@
       <c r="H65" s="38"/>
       <c r="I65" s="36"/>
     </row>
-    <row r="66" spans="1:9" ht="30">
+    <row r="66" spans="1:9" ht="30" hidden="1">
       <c r="A66" s="5"/>
       <c r="B66" s="5" t="s">
         <v>100</v>
@@ -2735,7 +2774,7 @@
       <c r="H66" s="38"/>
       <c r="I66" s="36"/>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" hidden="1">
       <c r="A67" s="5"/>
       <c r="B67" s="5" t="s">
         <v>101</v>
@@ -2756,19 +2795,19 @@
       <c r="H67" s="38"/>
       <c r="I67" s="36"/>
     </row>
-    <row r="68" spans="1:9" hidden="1">
+    <row r="68" spans="1:9">
       <c r="A68" s="30"/>
       <c r="B68" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="C68" s="2"/>
+      <c r="C68" s="30"/>
       <c r="D68" s="31" t="s">
         <v>212</v>
       </c>
       <c r="E68" s="25">
         <v>2</v>
       </c>
-      <c r="F68" s="2">
+      <c r="F68" s="30">
         <v>2</v>
       </c>
       <c r="G68" s="40" t="s">
@@ -2777,19 +2816,19 @@
       <c r="H68" s="38"/>
       <c r="I68" s="36"/>
     </row>
-    <row r="69" spans="1:9" hidden="1">
+    <row r="69" spans="1:9">
       <c r="A69" s="30"/>
       <c r="B69" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="C69" s="2"/>
+      <c r="C69" s="30"/>
       <c r="D69" s="30" t="s">
         <v>212</v>
       </c>
       <c r="E69" s="25">
         <v>2</v>
       </c>
-      <c r="F69" s="2">
+      <c r="F69" s="30">
         <v>3</v>
       </c>
       <c r="G69" s="40" t="s">
@@ -2798,21 +2837,21 @@
       <c r="H69" s="38"/>
       <c r="I69" s="36"/>
     </row>
-    <row r="70" spans="1:9" ht="21" hidden="1" customHeight="1">
+    <row r="70" spans="1:9" ht="21" customHeight="1">
       <c r="A70" s="30" t="s">
         <v>104</v>
       </c>
       <c r="B70" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="C70" s="2"/>
+      <c r="C70" s="30"/>
       <c r="D70" s="31" t="s">
         <v>212</v>
       </c>
       <c r="E70" s="25">
         <v>2</v>
       </c>
-      <c r="F70" s="2">
+      <c r="F70" s="30">
         <v>2</v>
       </c>
       <c r="G70" s="40" t="s">
@@ -2821,19 +2860,19 @@
       <c r="H70" s="38"/>
       <c r="I70" s="36"/>
     </row>
-    <row r="71" spans="1:9" hidden="1">
+    <row r="71" spans="1:9">
       <c r="A71" s="30"/>
       <c r="B71" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="C71" s="2"/>
+      <c r="C71" s="30"/>
       <c r="D71" s="31" t="s">
         <v>212</v>
       </c>
       <c r="E71" s="25">
         <v>2</v>
       </c>
-      <c r="F71" s="2">
+      <c r="F71" s="30">
         <v>2</v>
       </c>
       <c r="G71" s="40" t="s">
@@ -2842,19 +2881,19 @@
       <c r="H71" s="38"/>
       <c r="I71" s="36"/>
     </row>
-    <row r="72" spans="1:9" hidden="1">
+    <row r="72" spans="1:9">
       <c r="A72" s="30"/>
       <c r="B72" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="C72" s="2"/>
+      <c r="C72" s="30"/>
       <c r="D72" s="31" t="s">
         <v>212</v>
       </c>
       <c r="E72" s="25">
         <v>2</v>
       </c>
-      <c r="F72" s="2">
+      <c r="F72" s="30">
         <v>2</v>
       </c>
       <c r="G72" s="40" t="s">
@@ -2863,7 +2902,7 @@
       <c r="H72" s="38"/>
       <c r="I72" s="36"/>
     </row>
-    <row r="73" spans="1:9" customFormat="1" hidden="1">
+    <row r="73" spans="1:9" customFormat="1" ht="165" hidden="1">
       <c r="A73" s="1" t="s">
         <v>108</v>
       </c>
@@ -2928,26 +2967,26 @@
       <c r="H75" s="3"/>
       <c r="I75" s="8"/>
     </row>
-    <row r="76" spans="1:9" hidden="1">
+    <row r="76" spans="1:9">
       <c r="A76" s="30"/>
       <c r="B76" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="C76" s="2"/>
+      <c r="C76" s="30"/>
       <c r="D76" s="40" t="s">
         <v>212</v>
       </c>
       <c r="E76" s="25">
         <v>3</v>
       </c>
-      <c r="F76" s="2">
+      <c r="F76" s="30">
         <v>2</v>
       </c>
       <c r="G76" s="39"/>
       <c r="H76" s="38"/>
       <c r="I76" s="36"/>
     </row>
-    <row r="77" spans="1:9" customFormat="1" hidden="1">
+    <row r="77" spans="1:9" customFormat="1" ht="270" hidden="1">
       <c r="A77" s="1" t="s">
         <v>113</v>
       </c>
@@ -2970,7 +3009,7 @@
       <c r="H77" s="3"/>
       <c r="I77" s="8"/>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" hidden="1">
       <c r="A78" s="5"/>
       <c r="B78" s="5" t="s">
         <v>116</v>
@@ -2991,7 +3030,7 @@
       <c r="H78" s="38"/>
       <c r="I78" s="36"/>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:9" hidden="1">
       <c r="A79" s="5"/>
       <c r="B79" s="5" t="s">
         <v>117</v>
@@ -3096,7 +3135,7 @@
       <c r="H83" s="3"/>
       <c r="I83" s="8"/>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:9" hidden="1">
       <c r="A84" s="5"/>
       <c r="B84" s="5" t="s">
         <v>126</v>
@@ -3117,21 +3156,21 @@
       <c r="H84" s="38"/>
       <c r="I84" s="36"/>
     </row>
-    <row r="85" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="85" spans="1:9" ht="14.25" customHeight="1">
       <c r="A85" s="30" t="s">
         <v>127</v>
       </c>
       <c r="B85" s="30" t="s">
         <v>128</v>
       </c>
-      <c r="C85" s="6"/>
+      <c r="C85" s="30"/>
       <c r="D85" s="31" t="s">
         <v>212</v>
       </c>
       <c r="E85" s="24">
         <v>2</v>
       </c>
-      <c r="F85" s="6">
+      <c r="F85" s="30">
         <v>1</v>
       </c>
       <c r="G85" s="40" t="s">
@@ -3161,21 +3200,21 @@
       <c r="H86" s="3"/>
       <c r="I86" s="8"/>
     </row>
-    <row r="87" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="87" spans="1:9" ht="14.25" customHeight="1">
       <c r="A87" s="30" t="s">
         <v>131</v>
       </c>
       <c r="B87" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="C87" s="14"/>
+      <c r="C87" s="30"/>
       <c r="D87" s="31" t="s">
         <v>212</v>
       </c>
       <c r="E87" s="26">
         <v>3</v>
       </c>
-      <c r="F87" s="14">
+      <c r="F87" s="30">
         <v>2</v>
       </c>
       <c r="G87" s="40" t="s">
@@ -3184,7 +3223,7 @@
       <c r="H87" s="38"/>
       <c r="I87" s="36"/>
     </row>
-    <row r="88" spans="1:9">
+    <row r="88" spans="1:9" hidden="1">
       <c r="A88" s="5"/>
       <c r="B88" s="5" t="s">
         <v>133</v>
@@ -3205,7 +3244,7 @@
       <c r="H88" s="38"/>
       <c r="I88" s="36"/>
     </row>
-    <row r="89" spans="1:9" customFormat="1" hidden="1">
+    <row r="89" spans="1:9" customFormat="1" ht="405" hidden="1">
       <c r="A89" s="1" t="s">
         <v>134</v>
       </c>
@@ -3264,7 +3303,7 @@
       <c r="H91" s="3"/>
       <c r="I91" s="8"/>
     </row>
-    <row r="92" spans="1:9">
+    <row r="92" spans="1:9" hidden="1">
       <c r="A92" s="5"/>
       <c r="B92" s="5" t="s">
         <v>138</v>
@@ -3285,16 +3324,18 @@
       <c r="H92" s="38"/>
       <c r="I92" s="36"/>
     </row>
-    <row r="93" spans="1:9" hidden="1">
+    <row r="93" spans="1:9" ht="18.75" customHeight="1">
       <c r="A93" s="30" t="s">
         <v>139</v>
       </c>
       <c r="B93" s="30" t="s">
         <v>140</v>
       </c>
-      <c r="C93" s="30"/>
+      <c r="C93" s="30" t="s">
+        <v>237</v>
+      </c>
       <c r="D93" s="31" t="s">
-        <v>212</v>
+        <v>9</v>
       </c>
       <c r="E93" s="32">
         <v>2</v>
@@ -3306,45 +3347,49 @@
       <c r="H93" s="38"/>
       <c r="I93" s="36"/>
     </row>
-    <row r="94" spans="1:9" hidden="1">
+    <row r="94" spans="1:9">
       <c r="A94" s="30"/>
       <c r="B94" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="C94" s="2"/>
+      <c r="C94" s="30" t="s">
+        <v>238</v>
+      </c>
       <c r="D94" s="31" t="s">
-        <v>212</v>
+        <v>9</v>
       </c>
       <c r="E94" s="25">
         <v>2</v>
       </c>
-      <c r="F94" s="2">
+      <c r="F94" s="30">
         <v>2</v>
       </c>
       <c r="G94" s="30"/>
       <c r="H94" s="38"/>
       <c r="I94" s="36"/>
     </row>
-    <row r="95" spans="1:9" hidden="1">
+    <row r="95" spans="1:9" ht="14.25" customHeight="1">
       <c r="A95" s="30"/>
       <c r="B95" s="30" t="s">
         <v>142</v>
       </c>
-      <c r="C95" s="2"/>
+      <c r="C95" s="30" t="s">
+        <v>239</v>
+      </c>
       <c r="D95" s="31" t="s">
         <v>212</v>
       </c>
       <c r="E95" s="25">
         <v>2</v>
       </c>
-      <c r="F95" s="2">
+      <c r="F95" s="30">
         <v>2</v>
       </c>
       <c r="G95" s="30"/>
       <c r="H95" s="38"/>
       <c r="I95" s="36"/>
     </row>
-    <row r="96" spans="1:9">
+    <row r="96" spans="1:9" ht="12.75" hidden="1" customHeight="1">
       <c r="A96" s="5"/>
       <c r="B96" s="5" t="s">
         <v>143</v>
@@ -3365,57 +3410,59 @@
       <c r="H96" s="38"/>
       <c r="I96" s="36"/>
     </row>
-    <row r="97" spans="1:9" hidden="1">
+    <row r="97" spans="1:9">
       <c r="A97" s="30"/>
       <c r="B97" s="30" t="s">
         <v>144</v>
       </c>
-      <c r="C97" s="2"/>
+      <c r="C97" s="30"/>
       <c r="D97" s="31" t="s">
         <v>212</v>
       </c>
       <c r="E97" s="25">
         <v>2</v>
       </c>
-      <c r="F97" s="2">
+      <c r="F97" s="30">
         <v>2</v>
       </c>
       <c r="G97" s="30"/>
       <c r="H97" s="38"/>
       <c r="I97" s="36"/>
     </row>
-    <row r="98" spans="1:9" hidden="1">
+    <row r="98" spans="1:9">
       <c r="A98" s="30"/>
       <c r="B98" s="30" t="s">
         <v>145</v>
       </c>
-      <c r="C98" s="2"/>
-      <c r="D98" s="31" t="s">
-        <v>212</v>
+      <c r="C98" s="44" t="s">
+        <v>240</v>
+      </c>
+      <c r="D98" s="45" t="s">
+        <v>9</v>
       </c>
       <c r="E98" s="25">
         <v>2</v>
       </c>
-      <c r="F98" s="2">
+      <c r="F98" s="30">
         <v>2</v>
       </c>
       <c r="G98" s="30"/>
       <c r="H98" s="38"/>
       <c r="I98" s="36"/>
     </row>
-    <row r="99" spans="1:9" hidden="1">
+    <row r="99" spans="1:9">
       <c r="A99" s="30"/>
       <c r="B99" s="30" t="s">
         <v>146</v>
       </c>
-      <c r="C99" s="6"/>
+      <c r="C99" s="30"/>
       <c r="D99" s="31" t="s">
         <v>212</v>
       </c>
       <c r="E99" s="24">
         <v>3</v>
       </c>
-      <c r="F99" s="6">
+      <c r="F99" s="30">
         <v>2</v>
       </c>
       <c r="G99" s="40" t="s">
@@ -3424,7 +3471,7 @@
       <c r="H99" s="38"/>
       <c r="I99" s="36"/>
     </row>
-    <row r="100" spans="1:9">
+    <row r="100" spans="1:9" hidden="1">
       <c r="A100" s="5"/>
       <c r="B100" s="5" t="s">
         <v>147</v>
@@ -3445,26 +3492,26 @@
       <c r="H100" s="38"/>
       <c r="I100" s="36"/>
     </row>
-    <row r="101" spans="1:9" hidden="1">
+    <row r="101" spans="1:9">
       <c r="A101" s="30"/>
       <c r="B101" s="30" t="s">
         <v>148</v>
       </c>
-      <c r="C101" s="6"/>
+      <c r="C101" s="30"/>
       <c r="D101" s="31" t="s">
         <v>212</v>
       </c>
       <c r="E101" s="24">
         <v>2</v>
       </c>
-      <c r="F101" s="6">
+      <c r="F101" s="30">
         <v>2</v>
       </c>
       <c r="G101" s="39"/>
       <c r="H101" s="38"/>
       <c r="I101" s="36"/>
     </row>
-    <row r="102" spans="1:9">
+    <row r="102" spans="1:9" hidden="1">
       <c r="A102" s="5"/>
       <c r="B102" s="5" t="s">
         <v>149</v>
@@ -3485,7 +3532,7 @@
       <c r="H102" s="38"/>
       <c r="I102" s="36"/>
     </row>
-    <row r="103" spans="1:9" ht="15.75" customHeight="1">
+    <row r="103" spans="1:9" ht="15.75" hidden="1" customHeight="1">
       <c r="A103" s="5" t="s">
         <v>150</v>
       </c>
@@ -3508,7 +3555,7 @@
       <c r="H103" s="38"/>
       <c r="I103" s="36"/>
     </row>
-    <row r="104" spans="1:9" ht="17.25" customHeight="1">
+    <row r="104" spans="1:9" ht="17.25" hidden="1" customHeight="1">
       <c r="A104" s="5" t="s">
         <v>152</v>
       </c>
@@ -3531,7 +3578,7 @@
       <c r="H104" s="38"/>
       <c r="I104" s="36"/>
     </row>
-    <row r="105" spans="1:9">
+    <row r="105" spans="1:9" hidden="1">
       <c r="A105" s="5"/>
       <c r="B105" s="5" t="s">
         <v>154</v>
@@ -3552,7 +3599,7 @@
       <c r="H105" s="38"/>
       <c r="I105" s="36"/>
     </row>
-    <row r="106" spans="1:9" customFormat="1" hidden="1">
+    <row r="106" spans="1:9" customFormat="1" ht="270" hidden="1">
       <c r="A106" s="1" t="s">
         <v>155</v>
       </c>
@@ -3575,7 +3622,7 @@
       <c r="H106" s="3"/>
       <c r="I106" s="8"/>
     </row>
-    <row r="107" spans="1:9" customFormat="1" ht="30" hidden="1">
+    <row r="107" spans="1:9" customFormat="1" hidden="1">
       <c r="A107" s="1"/>
       <c r="B107" s="2" t="s">
         <v>157</v>
@@ -3596,7 +3643,7 @@
       <c r="H107" s="3"/>
       <c r="I107" s="8"/>
     </row>
-    <row r="108" spans="1:9">
+    <row r="108" spans="1:9" hidden="1">
       <c r="A108" s="5"/>
       <c r="B108" s="5" t="s">
         <v>159</v>
@@ -3617,7 +3664,7 @@
       <c r="H108" s="38"/>
       <c r="I108" s="36"/>
     </row>
-    <row r="109" spans="1:9" ht="18" customHeight="1">
+    <row r="109" spans="1:9" ht="18" hidden="1" customHeight="1">
       <c r="A109" s="5" t="s">
         <v>174</v>
       </c>
@@ -3638,7 +3685,7 @@
       <c r="H109" s="38"/>
       <c r="I109" s="36"/>
     </row>
-    <row r="110" spans="1:9">
+    <row r="110" spans="1:9" hidden="1">
       <c r="A110" s="5"/>
       <c r="B110" s="5" t="s">
         <v>176</v>
@@ -3657,7 +3704,7 @@
       <c r="H110" s="38"/>
       <c r="I110" s="36"/>
     </row>
-    <row r="111" spans="1:9">
+    <row r="111" spans="1:9" hidden="1">
       <c r="A111" s="5"/>
       <c r="B111" s="5" t="s">
         <v>177</v>
@@ -3676,7 +3723,7 @@
       <c r="H111" s="38"/>
       <c r="I111" s="36"/>
     </row>
-    <row r="112" spans="1:9">
+    <row r="112" spans="1:9" hidden="1">
       <c r="A112" s="5"/>
       <c r="B112" s="5" t="s">
         <v>178</v>
@@ -3695,7 +3742,7 @@
       <c r="H112" s="38"/>
       <c r="I112" s="36"/>
     </row>
-    <row r="113" spans="1:9">
+    <row r="113" spans="1:9" hidden="1">
       <c r="A113" s="5"/>
       <c r="B113" s="5" t="s">
         <v>179</v>
@@ -3714,7 +3761,7 @@
       <c r="H113" s="38"/>
       <c r="I113" s="36"/>
     </row>
-    <row r="114" spans="1:9">
+    <row r="114" spans="1:9" hidden="1">
       <c r="A114" s="5"/>
       <c r="B114" s="5" t="s">
         <v>180</v>
@@ -3733,7 +3780,7 @@
       <c r="H114" s="38"/>
       <c r="I114" s="36"/>
     </row>
-    <row r="115" spans="1:9">
+    <row r="115" spans="1:9" hidden="1">
       <c r="A115" s="5"/>
       <c r="B115" s="5" t="s">
         <v>181</v>
@@ -3752,40 +3799,44 @@
       <c r="H115" s="38"/>
       <c r="I115" s="36"/>
     </row>
-    <row r="116" spans="1:9" ht="16.5" hidden="1" customHeight="1">
+    <row r="116" spans="1:9" ht="16.5" customHeight="1">
       <c r="A116" s="30" t="s">
         <v>160</v>
       </c>
       <c r="B116" s="30" t="s">
         <v>161</v>
       </c>
-      <c r="C116" s="6"/>
+      <c r="C116" s="30" t="s">
+        <v>236</v>
+      </c>
       <c r="D116" s="31" t="s">
-        <v>212</v>
+        <v>9</v>
       </c>
       <c r="E116" s="24">
         <v>0</v>
       </c>
-      <c r="F116" s="6">
+      <c r="F116" s="30">
         <v>0</v>
       </c>
       <c r="G116" s="39"/>
       <c r="H116" s="38"/>
       <c r="I116" s="36"/>
     </row>
-    <row r="117" spans="1:9" hidden="1">
+    <row r="117" spans="1:9">
       <c r="A117" s="30"/>
       <c r="B117" s="30" t="s">
         <v>162</v>
       </c>
-      <c r="C117" s="6"/>
+      <c r="C117" s="30" t="s">
+        <v>235</v>
+      </c>
       <c r="D117" s="31" t="s">
-        <v>212</v>
+        <v>9</v>
       </c>
       <c r="E117" s="24">
         <v>0</v>
       </c>
-      <c r="F117" s="6">
+      <c r="F117" s="30">
         <v>0</v>
       </c>
       <c r="G117" s="39"/>
@@ -3834,26 +3885,26 @@
       <c r="H119" s="3"/>
       <c r="I119" s="8"/>
     </row>
-    <row r="120" spans="1:9" hidden="1">
+    <row r="120" spans="1:9">
       <c r="A120" s="30"/>
       <c r="B120" s="30" t="s">
         <v>165</v>
       </c>
-      <c r="C120" s="6"/>
+      <c r="C120" s="30"/>
       <c r="D120" s="28" t="s">
         <v>212</v>
       </c>
       <c r="E120" s="24">
         <v>1</v>
       </c>
-      <c r="F120" s="6">
+      <c r="F120" s="30">
         <v>2</v>
       </c>
       <c r="G120" s="30"/>
       <c r="H120" s="38"/>
       <c r="I120" s="36"/>
     </row>
-    <row r="121" spans="1:9">
+    <row r="121" spans="1:9" hidden="1">
       <c r="A121" s="30"/>
       <c r="B121" s="5" t="s">
         <v>166</v>
@@ -3874,7 +3925,7 @@
       <c r="H121" s="38"/>
       <c r="I121" s="36"/>
     </row>
-    <row r="122" spans="1:9">
+    <row r="122" spans="1:9" hidden="1">
       <c r="A122" s="5"/>
       <c r="B122" s="5" t="s">
         <v>167</v>
@@ -3895,7 +3946,7 @@
       <c r="H122" s="38"/>
       <c r="I122" s="36"/>
     </row>
-    <row r="123" spans="1:9">
+    <row r="123" spans="1:9" hidden="1">
       <c r="A123" s="5"/>
       <c r="B123" s="5" t="s">
         <v>168</v>
@@ -3937,7 +3988,7 @@
       <c r="H124" s="3"/>
       <c r="I124" s="8"/>
     </row>
-    <row r="125" spans="1:9">
+    <row r="125" spans="1:9" hidden="1">
       <c r="A125" s="5"/>
       <c r="B125" s="5" t="s">
         <v>170</v>
@@ -3977,7 +4028,7 @@
       <c r="H126" s="3"/>
       <c r="I126" s="8"/>
     </row>
-    <row r="127" spans="1:9" customFormat="1" hidden="1">
+    <row r="127" spans="1:9" customFormat="1" ht="180" hidden="1">
       <c r="A127" s="1"/>
       <c r="B127" s="2" t="s">
         <v>171</v>
@@ -3998,19 +4049,19 @@
       <c r="H127" s="3"/>
       <c r="I127" s="8"/>
     </row>
-    <row r="128" spans="1:9" hidden="1">
+    <row r="128" spans="1:9">
       <c r="A128" s="30"/>
       <c r="B128" s="30" t="s">
         <v>172</v>
       </c>
-      <c r="C128" s="2"/>
+      <c r="C128" s="30"/>
       <c r="D128" s="31" t="s">
         <v>212</v>
       </c>
       <c r="E128" s="25">
         <v>2</v>
       </c>
-      <c r="F128" s="2">
+      <c r="F128" s="30">
         <v>2</v>
       </c>
       <c r="G128" s="30" t="s">
@@ -4019,7 +4070,7 @@
       <c r="H128" s="38"/>
       <c r="I128" s="36"/>
     </row>
-    <row r="129" spans="1:9">
+    <row r="129" spans="1:9" hidden="1">
       <c r="A129" s="5"/>
       <c r="B129" s="5" t="s">
         <v>183</v>
@@ -4040,7 +4091,7 @@
       <c r="H129" s="38"/>
       <c r="I129" s="36"/>
     </row>
-    <row r="130" spans="1:9">
+    <row r="130" spans="1:9" hidden="1">
       <c r="A130" s="5"/>
       <c r="B130" s="5" t="s">
         <v>184</v>
@@ -4082,7 +4133,7 @@
       <c r="H131" s="3"/>
       <c r="I131" s="8"/>
     </row>
-    <row r="132" spans="1:9" customFormat="1" hidden="1">
+    <row r="132" spans="1:9" customFormat="1" ht="135" hidden="1">
       <c r="A132" s="1"/>
       <c r="B132" s="2" t="s">
         <v>186</v>
@@ -4103,7 +4154,7 @@
       <c r="H132" s="3"/>
       <c r="I132" s="8"/>
     </row>
-    <row r="133" spans="1:9">
+    <row r="133" spans="1:9" hidden="1">
       <c r="A133" s="5"/>
       <c r="B133" s="5" t="s">
         <v>187</v>
@@ -4124,7 +4175,7 @@
       <c r="H133" s="38"/>
       <c r="I133" s="36"/>
     </row>
-    <row r="134" spans="1:9">
+    <row r="134" spans="1:9" hidden="1">
       <c r="A134" s="5"/>
       <c r="B134" s="5" t="s">
         <v>188</v>
@@ -4145,49 +4196,53 @@
       <c r="H134" s="38"/>
       <c r="I134" s="36"/>
     </row>
-    <row r="135" spans="1:9" hidden="1">
+    <row r="135" spans="1:9">
       <c r="A135" s="30"/>
       <c r="B135" s="30" t="s">
         <v>189</v>
       </c>
-      <c r="C135" s="2"/>
+      <c r="C135" s="30"/>
       <c r="D135" s="31" t="s">
         <v>212</v>
       </c>
       <c r="E135" s="25">
         <v>1</v>
       </c>
-      <c r="F135" s="2">
+      <c r="F135" s="30">
         <v>3</v>
       </c>
       <c r="G135" s="30"/>
       <c r="H135" s="38"/>
       <c r="I135" s="36"/>
     </row>
-    <row r="136" spans="1:9" hidden="1">
+    <row r="136" spans="1:9">
       <c r="A136" s="30"/>
       <c r="B136" s="30" t="s">
         <v>190</v>
       </c>
-      <c r="C136" s="2"/>
+      <c r="C136" s="30"/>
       <c r="D136" s="31" t="s">
         <v>212</v>
       </c>
       <c r="E136" s="25">
         <v>2</v>
       </c>
-      <c r="F136" s="2">
+      <c r="F136" s="30">
         <v>2</v>
       </c>
       <c r="G136" s="30"/>
       <c r="H136" s="38"/>
       <c r="I136" s="36"/>
+    </row>
+    <row r="137" spans="1:9">
+      <c r="C137" s="37"/>
+      <c r="F137" s="37"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F136" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="3">
       <filters>
-        <filter val="N/A"/>
+        <filter val="Planning"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>